<commit_message>
updating to include formatting for second loop table (not done yet)
</commit_message>
<xml_diff>
--- a/loop-tables.xlsx
+++ b/loop-tables.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="460" windowWidth="20160" windowHeight="11480" tabRatio="500"/>
+    <workbookView xWindow="7900" yWindow="460" windowWidth="20160" windowHeight="11480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Loop Table 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Loop Table 2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Loop Table 1</t>
   </si>
@@ -51,6 +52,18 @@
   </si>
   <si>
     <t>the loop stops here, because 16 is less than or equal to 17; adding two to that for the next loop would result in x being greater than 17</t>
+  </si>
+  <si>
+    <t>Loop Table 2</t>
+  </si>
+  <si>
+    <t>value of index</t>
+  </si>
+  <si>
+    <t>value of s1</t>
+  </si>
+  <si>
+    <t>value of s2</t>
   </si>
 </sst>
 </file>
@@ -94,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -102,6 +115,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -149,6 +165,49 @@
         <a:xfrm>
           <a:off x="861786" y="215900"/>
           <a:ext cx="3824514" cy="787400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>722233</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="215900"/>
+          <a:ext cx="4176633" cy="2006600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -423,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,9 +647,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="6" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
maybe finished loop table 2
</commit_message>
<xml_diff>
--- a/loop-tables.xlsx
+++ b/loop-tables.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8600" yWindow="2780" windowWidth="20160" windowHeight="11480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="20160" windowHeight="11480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Loop Table 1" sheetId="1" r:id="rId1"/>
     <sheet name="Loop Table 2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>Loop Table 1</t>
   </si>
@@ -42,12 +42,6 @@
     <t>output</t>
   </si>
   <si>
-    <t>x starts at 0, and we display 2 * x + 7, which is 2 * 0 + 7  = 0 + 7 = 7 for the first loop</t>
-  </si>
-  <si>
-    <t>we add to to x, as per the x = x + 2 in the loop, and we repeat the 2 * x + 7, which is 11 in this case</t>
-  </si>
-  <si>
     <t>and so on</t>
   </si>
   <si>
@@ -64,6 +58,39 @@
   </si>
   <si>
     <t>value of s2</t>
+  </si>
+  <si>
+    <t>x starts at 0, and we display 2 * x + 7 in the console, which is 2 * 0 + 7  = 0 + 7 = 7 for the first loop</t>
+  </si>
+  <si>
+    <t>we add two to x, as per the x = x + 2 in the loop, and we repeat the 2 * x + 7, which is 11 in this case</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>''</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>index starts at 0, and the loop will continue as long as index is less than 8 (alpha.length);  if index divided by 2 results in a remainder of zero (meaning index is even), s1 is equal to s1 plus the string character that is the value of index, 1; if it's an odd number (modulo is not 0), s2 is equal to the value of s2 plus the string character that is the value of index, 1; at the end of every loop we'll add one to index; once we get to index equal to 7, display s1 + s2 in console</t>
   </si>
 </sst>
 </file>
@@ -107,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -118,6 +145,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -181,19 +214,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>10006</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>722233</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>191382</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -206,8 +239,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="914400" y="215900"/>
-          <a:ext cx="4176633" cy="2006600"/>
+          <a:off x="924406" y="63499"/>
+          <a:ext cx="4117494" cy="2363083"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -485,7 +518,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,7 +564,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -547,7 +580,7 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -563,7 +596,7 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -644,7 +677,7 @@
         <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -655,10 +688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -667,28 +700,168 @@
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" customWidth="1"/>
     <col min="4" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="77.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="1">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="1">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="1">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="1">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1">
+        <v>7</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding more explanation for loop table 2
</commit_message>
<xml_diff>
--- a/loop-tables.xlsx
+++ b/loop-tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="20160" windowHeight="11480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7780" yWindow="3560" windowWidth="20160" windowHeight="11480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Loop Table 1" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
     <t>w</t>
   </si>
   <si>
-    <t>index starts at 0, and the loop will continue as long as index is less than 8 (alpha.length);  if index divided by 2 results in a remainder of zero (meaning index is even), s1 is equal to s1 plus the string character that is the value of index, 1; if it's an odd number (modulo is not 0), s2 is equal to the value of s2 plus the string character that is the value of index, 1; at the end of every loop we'll add one to index; once we get to index equal to 7, display s1 + s2 in console</t>
+    <t>index starts at 0, and the loop will continue as long as index is less than 8 (alpha.length);  if index divided by 2 results in a remainder of zero (meaning index is even), s1 is equal to s1 plus the string character that is the value of index, 1; if it's an odd number (modulo is not 0), s2 is equal to the value of s2 plus the string character that is the value of index, 1; at the end of every loop we'll add one to index; since we set variables that were blank for s1 and s2, the JS will store everything we put into them until the condition is no longer true (index &gt; alpha.length), and then it will display s1 + s2 in console --&gt; meowpurr</t>
   </si>
 </sst>
 </file>
@@ -690,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,7 +725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
adjustments to table and explanation
</commit_message>
<xml_diff>
--- a/loop-tables.xlsx
+++ b/loop-tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="3560" windowWidth="20160" windowHeight="11480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8520" yWindow="3240" windowWidth="22520" windowHeight="12740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Loop Table 1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>Loop Table 1</t>
   </si>
@@ -72,25 +72,28 @@
     <t>''</t>
   </si>
   <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>p</t>
   </si>
   <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>index starts at 0, and the loop will continue as long as index is less than 8 (alpha.length);  if index divided by 2 results in a remainder of zero (meaning index is even), s1 is equal to s1 plus the string character that is the value of index, 1; if it's an odd number (modulo is not 0), s2 is equal to the value of s2 plus the string character that is the value of index, 1; at the end of every loop we'll add one to index; since we set variables that were blank for s1 and s2, the JS will store everything we put into them until the condition is no longer true (index &gt; alpha.length), and then it will display s1 + s2 in console --&gt; meowpurr</t>
+    <t>me</t>
+  </si>
+  <si>
+    <t>pu</t>
+  </si>
+  <si>
+    <t>meo</t>
+  </si>
+  <si>
+    <t>pur</t>
+  </si>
+  <si>
+    <t>meow</t>
+  </si>
+  <si>
+    <t>purr</t>
+  </si>
+  <si>
+    <t>index starts at 0, and the loop will continue as long as index is less than 8 (alpha.length);  if index divided by 2 results in a remainder of zero (meaning index is even), s1 is equal to s1 plus the string character that is the value of index, 1; if it's an odd number (modulo is not 0), s2 is equal to the value of s2 plus the string character that is the value of index, 1; at the end of every loop we'll add one to index; when the condition is no longer true (when index &gt; alpha.length), and then it will display s1 + s2 in console --&gt; "meow" + "purr" = meowpurr</t>
   </si>
 </sst>
 </file>
@@ -690,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,7 +728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>1</v>
       </c>
@@ -742,7 +745,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -756,10 +759,10 @@
         <v>13</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -770,13 +773,13 @@
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -858,10 +861,10 @@
         <v>13</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
couple quick edits to each table
</commit_message>
<xml_diff>
--- a/loop-tables.xlsx
+++ b/loop-tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="3240" windowWidth="22520" windowHeight="12740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6280" yWindow="3240" windowWidth="22520" windowHeight="12740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Loop Table 1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Loop Table 1</t>
   </si>
@@ -45,9 +45,6 @@
     <t>and so on</t>
   </si>
   <si>
-    <t>the loop stops here, because 16 is less than or equal to 17; adding two to that for the next loop would result in x being greater than 17</t>
-  </si>
-  <si>
     <t>Loop Table 2</t>
   </si>
   <si>
@@ -94,6 +91,12 @@
   </si>
   <si>
     <t>index starts at 0, and the loop will continue as long as index is less than 8 (alpha.length);  if index divided by 2 results in a remainder of zero (meaning index is even), s1 is equal to s1 plus the string character that is the value of index, 1; if it's an odd number (modulo is not 0), s2 is equal to the value of s2 plus the string character that is the value of index, 1; at the end of every loop we'll add one to index; when the condition is no longer true (when index &gt; alpha.length),  it will display s1 + s2 in console --&gt; "meow" + "purr" = meowpurr</t>
+  </si>
+  <si>
+    <t>the loop stops here, because 18 is not less than or equal to 17</t>
+  </si>
+  <si>
+    <t>meowpurr</t>
   </si>
 </sst>
 </file>
@@ -137,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -155,6 +158,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,7 +574,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -583,7 +590,7 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -679,8 +686,16 @@
         <f>2 *C15 +7</f>
         <v>39</v>
       </c>
-      <c r="E15" t="s">
-        <v>5</v>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>10</v>
+      </c>
+      <c r="C16" s="4">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -691,10 +706,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -708,7 +723,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -716,13 +731,13 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>3</v>
@@ -736,16 +751,16 @@
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -756,13 +771,13 @@
         <v>1</v>
       </c>
       <c r="D15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -773,13 +788,13 @@
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -790,13 +805,13 @@
         <v>3</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
@@ -807,13 +822,13 @@
         <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
@@ -824,13 +839,13 @@
         <v>5</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
@@ -841,13 +856,13 @@
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
@@ -858,16 +873,35 @@
         <v>7</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="1">
+        <v>9</v>
+      </c>
+      <c r="C22" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="E24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E24:F24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>